<commit_message>
refactor: the logic class structure in xml files
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Buff.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Buff.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherish\Desktop\git\nf\develop\_Out\Server\NFDataCfg\Excel_Ini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Desktop\NoahGameFrame\_Out\NFDataCfg\Excel_Ini\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27520" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="27518" windowHeight="17543"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Id</t>
   </si>
@@ -128,14 +128,16 @@
   </si>
   <si>
     <t>Upload</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Force</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -350,7 +352,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
@@ -694,28 +696,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" customWidth="1"/>
-    <col min="4" max="4" width="22.6328125" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" customWidth="1"/>
-    <col min="6" max="6" width="20.453125" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" customWidth="1"/>
-    <col min="8" max="8" width="18.36328125" customWidth="1"/>
-    <col min="9" max="9" width="19.36328125" customWidth="1"/>
-    <col min="10" max="10" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="10.46484375" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.19921875" customWidth="1"/>
+    <col min="4" max="4" width="22.59765625" customWidth="1"/>
+    <col min="5" max="5" width="17.19921875" customWidth="1"/>
+    <col min="6" max="6" width="20.46484375" customWidth="1"/>
+    <col min="7" max="7" width="12.59765625" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -747,7 +749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -779,7 +781,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="2" customFormat="1">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -811,7 +813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="2" customFormat="1">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -843,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="2" customFormat="1">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
@@ -875,7 +877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="2" customFormat="1">
       <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
@@ -907,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="3" customFormat="1">
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
@@ -939,105 +941,105 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="3" customFormat="1">
       <c r="A8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="3" customFormat="1">
+      <c r="A9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3" t="b">
+      <c r="B9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="10" spans="1:10" s="4" customFormat="1" ht="81">
+      <c r="A10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J10" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:10" s="5" customFormat="1">
+      <c r="A11" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5">
-        <v>1</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1</v>
-      </c>
-      <c r="I10" s="5">
-        <v>1</v>
-      </c>
-      <c r="J10" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>28</v>
@@ -1064,16 +1066,48 @@
         <v>1</v>
       </c>
       <c r="J11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="5" customFormat="1">
+      <c r="A12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:A8"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:J8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:J8 B8:J8 B9:AF9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:A9"/>
   </dataValidations>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>